<commit_message>
Updated Census Report Template to default to the Census Sheet
</commit_message>
<xml_diff>
--- a/static/Medical Census Roster Sheet_22OCT2023.xlsx
+++ b/static/Medical Census Roster Sheet_22OCT2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Amateur Radio\AREDN\MCM_2023\Medical Census Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/porcej/dev/2023mcm/med-tracker/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9E02079-2A2F-4519-A392-A23DE59CA4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D0B058-4592-C442-B5B5-AA03F8675007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Census Roster Sheet" sheetId="2" r:id="rId1"/>
@@ -468,6 +468,15 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -480,20 +489,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -783,36 +783,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF80147-7C11-41D5-BD77-CE20B6187366}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:3" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -821,216 +821,216 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="10"/>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="20"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="21"/>
+      <c r="C7" s="23"/>
+    </row>
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="21"/>
+      <c r="C8" s="23"/>
+    </row>
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="21"/>
+      <c r="C9" s="23"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+    </row>
+    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21"/>
+      <c r="C11" s="23"/>
+    </row>
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21"/>
+      <c r="C12" s="23"/>
+    </row>
+    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="20"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21"/>
+      <c r="C13" s="23"/>
+    </row>
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="23"/>
+    </row>
+    <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="21"/>
+      <c r="C15" s="23"/>
+    </row>
+    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="20"/>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="21"/>
+      <c r="C16" s="23"/>
+    </row>
+    <row r="17" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="20"/>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="21"/>
+      <c r="C19" s="23"/>
+    </row>
+    <row r="20" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="20"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="21"/>
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="20"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="21"/>
+      <c r="C21" s="23"/>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="20"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="21"/>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="20"/>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="21"/>
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21"/>
+      <c r="C24" s="23"/>
+    </row>
+    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="20"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="21"/>
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="20"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="23"/>
+    </row>
+    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="20"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="23"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="20"/>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="21"/>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="23"/>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="20"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="21"/>
+      <c r="C31" s="23"/>
+    </row>
+    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="20"/>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="21"/>
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="20"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="21"/>
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="20"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="21"/>
+      <c r="C34" s="23"/>
+    </row>
+    <row r="35" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="20"/>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="21"/>
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-    </row>
-    <row r="42" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+    </row>
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+    </row>
+    <row r="40" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+    </row>
+    <row r="42" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -1042,204 +1042,246 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="10"/>
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="21" t="s">
+    <row r="47" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+    </row>
+    <row r="48" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="20"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21"/>
+      <c r="C48" s="23"/>
+    </row>
+    <row r="49" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="20"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="21"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="20"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="21"/>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="20"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="21"/>
+      <c r="C51" s="23"/>
+    </row>
+    <row r="52" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="20"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="21"/>
+      <c r="C52" s="23"/>
+    </row>
+    <row r="53" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="20"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="21"/>
+      <c r="C53" s="23"/>
+    </row>
+    <row r="54" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="20"/>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="21"/>
+      <c r="C54" s="23"/>
+    </row>
+    <row r="55" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="20"/>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="21"/>
+      <c r="C55" s="23"/>
+    </row>
+    <row r="56" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="20"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="21"/>
+      <c r="C56" s="23"/>
+    </row>
+    <row r="57" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="20"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="21"/>
+      <c r="C57" s="23"/>
+    </row>
+    <row r="58" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="21" t="s">
+    <row r="59" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="23"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
+    </row>
+    <row r="60" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="20"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="21"/>
+      <c r="C60" s="23"/>
+    </row>
+    <row r="61" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="20"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="21"/>
+      <c r="C61" s="23"/>
+    </row>
+    <row r="62" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="20"/>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="21"/>
+      <c r="C62" s="23"/>
+    </row>
+    <row r="63" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="20"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="21"/>
+      <c r="C63" s="23"/>
+    </row>
+    <row r="64" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="20"/>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="21"/>
+      <c r="C64" s="23"/>
+    </row>
+    <row r="65" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="20"/>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="21"/>
+      <c r="C65" s="23"/>
+    </row>
+    <row r="66" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="20"/>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="21"/>
+      <c r="C66" s="23"/>
+    </row>
+    <row r="67" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="20"/>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="21"/>
+      <c r="C67" s="23"/>
+    </row>
+    <row r="68" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="20"/>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="21"/>
+      <c r="C68" s="23"/>
+    </row>
+    <row r="69" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="20"/>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="21"/>
+      <c r="C69" s="23"/>
+    </row>
+    <row r="70" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C71" s="23"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="20"/>
+    </row>
+    <row r="72" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="20"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="21"/>
+      <c r="C72" s="23"/>
+    </row>
+    <row r="73" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="20"/>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="21"/>
+      <c r="C73" s="23"/>
+    </row>
+    <row r="74" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="20"/>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="21"/>
+      <c r="C74" s="23"/>
+    </row>
+    <row r="75" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="20"/>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="21"/>
+      <c r="C75" s="23"/>
+    </row>
+    <row r="76" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
-      <c r="B76" s="18"/>
-      <c r="C76" s="20"/>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="21"/>
+      <c r="C76" s="23"/>
+    </row>
+    <row r="77" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
     </row>
-    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
+    <row r="78" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="23"/>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="20"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20"/>
+    </row>
+    <row r="79" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+    </row>
+    <row r="80" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="23"/>
+    </row>
+    <row r="81" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="23"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ak5nWml53ofn5rhwFzgoHNw8JtgdPMKqpBKIDFJwBJGBkBRa+wIAk/eIduTU9jSL8v/Gh3uE91gdDxCv3MXSQQ==" saltValue="syi1YFRudrq7nhXOsXYirA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="68">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A39:C39"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B25:C25"/>
@@ -1256,53 +1298,11 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="A78:C78"/>
-    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1317,50 +1317,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DF4227-963E-499B-AD1E-E89C147203B8}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="27"/>
     </row>
-    <row r="2" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="26"/>
     </row>
-    <row r="3" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="26"/>
     </row>
-    <row r="4" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="26"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+    </row>
+    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1472,43 +1472,43 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="26"/>
     </row>
-    <row r="24" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="26"/>
     </row>
-    <row r="25" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="26"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="23"/>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="20"/>
+    </row>
+    <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>44</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>46</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
     </row>
   </sheetData>
@@ -1573,12 +1573,12 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>

</xml_diff>